<commit_message>
generate script to rename figures
</commit_message>
<xml_diff>
--- a/fig/fig_names.xlsx
+++ b/fig/fig_names.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15860" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="deterministic_evo" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>fig_name</t>
   </si>
@@ -37,9 +37,6 @@
     <t>chapter</t>
   </si>
   <si>
-    <t>library</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -49,7 +46,31 @@
     <t>deterministic_mut</t>
   </si>
   <si>
-    <t>mpl-bokeh</t>
+    <t>random_walk</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>buri_schematic</t>
+  </si>
+  <si>
+    <t>buri_generations</t>
+  </si>
+  <si>
+    <t>buri_experiment</t>
+  </si>
+  <si>
+    <t>ensemble_realization</t>
+  </si>
+  <si>
+    <t>average_langevin</t>
+  </si>
+  <si>
+    <t>chapman_kolmogorov</t>
+  </si>
+  <si>
+    <t>schematic_reverse</t>
   </si>
 </sst>
 </file>
@@ -366,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -383,7 +404,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -391,7 +412,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -399,13 +420,13 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -413,8 +434,8 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -424,13 +445,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -440,10 +464,94 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -453,13 +561,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -469,10 +580,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>